<commit_message>
website and val data new
</commit_message>
<xml_diff>
--- a/data/website_data/urls_website.xlsx
+++ b/data/website_data/urls_website.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Erasmus\Transformer_Pretraining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Erasmus\Transformer_Pretraining\Bounwiki\data\website_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D553F5-39F5-499B-8C05-CBD2B8481D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8FD87F-509A-455C-B333-A24F91AD81ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1620" windowWidth="17280" windowHeight="8964" xr2:uid="{62C1F806-0E46-4012-9DA9-47B75316CFBC}"/>
+    <workbookView xWindow="9036" yWindow="1080" windowWidth="6168" windowHeight="8964" xr2:uid="{62C1F806-0E46-4012-9DA9-47B75316CFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>Campuses</t>
   </si>
@@ -104,12 +104,6 @@
   </si>
   <si>
     <t>https://www.boun.edu.tr/en_US/Content/About_BU/History</t>
-  </si>
-  <si>
-    <t>Vision Mission</t>
-  </si>
-  <si>
-    <t>https://www.boun.edu.tr/en_US/Content/About_BU/Vision_Mission</t>
   </si>
   <si>
     <t>Academic Calendar</t>
@@ -660,16 +654,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A36EA7F-AEC4-4673-AC3F-95BF649376AC}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -790,7 +784,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -801,7 +795,7 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -812,18 +806,18 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -834,7 +828,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -845,7 +839,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -938,10 +932,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
         <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
@@ -949,10 +943,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
         <v>55</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
@@ -1087,7 +1081,7 @@
         <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1098,7 +1092,7 @@
         <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1120,17 +1114,6 @@
         <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>